<commit_message>
changed the columns name
</commit_message>
<xml_diff>
--- a/stimuli/arguments.xlsx
+++ b/stimuli/arguments.xlsx
@@ -582,13 +582,13 @@
     <t>La prugna contiene un albero</t>
   </si>
   <si>
-    <t>argumentP1</t>
-  </si>
-  <si>
-    <t>argumentP2</t>
-  </si>
-  <si>
-    <t>argumentC</t>
+    <t>premise1</t>
+  </si>
+  <si>
+    <t>premise2</t>
+  </si>
+  <si>
+    <t>conclusion</t>
   </si>
 </sst>
 </file>
@@ -987,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
updated the argument text
</commit_message>
<xml_diff>
--- a/stimuli/arguments.xlsx
+++ b/stimuli/arguments.xlsx
@@ -10,6 +10,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="arg" localSheetId="0">Sheet1!#REF!</definedName>
+    <definedName name="arg_copy_2" localSheetId="0">Sheet1!$G$2:$I$81</definedName>
     <definedName name="arguments" localSheetId="0">Sheet1!$A$1:$J$81</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -23,8 +25,35 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="arguments.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:antonio:Desktop:arguments.txt" decimal="," thousands="." tab="0" comma="1">
+  <connection id="1" name="arg copy 2.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr sourceFile="Macintosh HD:Users:francesca:Desktop:arg copy 2.txt" tab="0" delimiter="|">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="arg.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:francesca:Desktop:arg.txt" tab="0" delimiter="|">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="arg.txt1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:francesca:Desktop:arg.txt" tab="0" delimiter="|">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="arguments.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:antonio:Desktop:arguments.txt" decimal="," thousands="." tab="0" comma="1">
       <textFields count="7">
         <textField/>
         <textField/>
@@ -40,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="419">
   <si>
     <t>ArgumentBlock</t>
   </si>
@@ -75,39 +104,21 @@
     <t>N</t>
   </si>
   <si>
-    <t>La prugna contiene il ‚Ä¶ |Il ... √® un albero |La prugna contiene un albero</t>
-  </si>
-  <si>
     <t>NOCCIOLO</t>
   </si>
   <si>
-    <t>Una certa quantit√† √® un ... |Un ... scava buche |Una certa quantit√† scava buche</t>
-  </si>
-  <si>
     <t>TASSO</t>
   </si>
   <si>
-    <t>Fabrizio Corona √® un ... |Un ... √® un fiore |Fabrizio Corona √® un fiore</t>
-  </si>
-  <si>
     <t xml:space="preserve"> NARCISO</t>
   </si>
   <si>
-    <t>I capelli hanno un ... |Un ... √® un porcospino |I capelli hanno un porcospino</t>
-  </si>
-  <si>
     <t>RICCIO</t>
   </si>
   <si>
-    <t>Un capitombolo √® un ... |Un ... √® un nastro arrotolato |Un capitombolo √® un nastro arrotolato</t>
-  </si>
-  <si>
     <t xml:space="preserve"> ROTOLONE</t>
   </si>
   <si>
-    <t>La buccia √® uno ... |Uno ... √® una grossa differenza |La buccia √® una grossa differenza</t>
-  </si>
-  <si>
     <t xml:space="preserve"> SCARTO</t>
   </si>
   <si>
@@ -117,123 +128,66 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Il caseificio produce ... |... √® formaggio |Il caseificio produce formaggio</t>
-  </si>
-  <si>
     <t xml:space="preserve"> GRANA </t>
   </si>
   <si>
-    <t>La televisione √® un ... |Un ... √® molto diffuso |La televisione √® molto diffusa</t>
-  </si>
-  <si>
     <t xml:space="preserve"> MEDIA</t>
   </si>
   <si>
-    <t>La zia coltiva il ... |Il ... √® una pianta |La zia coltiva una pianta</t>
-  </si>
-  <si>
     <t>MIGLIO</t>
   </si>
   <si>
-    <t>Al bivio c'√® un ... |Un ... √® un'interruzione |Al bivio c'√® un'interruzione</t>
-  </si>
-  <si>
     <t xml:space="preserve"> BLOCCO</t>
   </si>
   <si>
-    <t>Belen √® una ... |Una ... √® una showgirl |Belen √® una showgirl</t>
-  </si>
-  <si>
     <t>VALLETTA</t>
   </si>
   <si>
-    <t>In montagna c‚Äô√® una ... |Una ... √® un piano inclinato |In montagna c‚Äô√® un piano inclinato</t>
-  </si>
-  <si>
     <t>SCARPATA</t>
   </si>
   <si>
     <t>TPPC</t>
   </si>
   <si>
-    <t>Una scommessa √® una ... |Una ... √® trasmessa in TV |Una scommessa √® trasmessa in TV</t>
-  </si>
-  <si>
     <t>PUNTATA</t>
   </si>
   <si>
-    <t>Un assortimento √® una ... |Una ... √® greca |Un assortimento √® greco</t>
-  </si>
-  <si>
     <t>GAMMA</t>
   </si>
   <si>
-    <t>Un portiere ha fatto una ... |Una ... √® una sfilata militare |Un portiere ha fatto una sfilata militare</t>
-  </si>
-  <si>
     <t>PARATA</t>
   </si>
   <si>
-    <t>La guardia forestale ha una ... |Una ... √® una somma illegale |La guardia forestale ha una somma illegale</t>
-  </si>
-  <si>
     <t>MAZZETTA</t>
   </si>
   <si>
-    <t>A Verona c'√® l'... |L'... √® sabbia |A Verona c'√® sabbia</t>
-  </si>
-  <si>
     <t>ARENA</t>
   </si>
   <si>
-    <t>Talete √® un ... |Un ... √® una lettura piacevole |Talete √® una lettura piacevole</t>
-  </si>
-  <si>
     <t>SAGGIO</t>
   </si>
   <si>
     <t>P</t>
   </si>
   <si>
-    <t>Un lingotto √® una ... |Una ... √® una lineetta |Un lingotto √® una lineetta</t>
-  </si>
-  <si>
     <t>BARRA</t>
   </si>
   <si>
-    <t>La luna forma uno ... |Uno ... √® una parte del frutto |La luna forma una parte del frutto</t>
-  </si>
-  <si>
     <t>SPICCHIO</t>
   </si>
   <si>
-    <t>Il nuotatore percorre una ... |Una ... √® una sezione stradale |Il nuotatore percorre una sezione stradale</t>
-  </si>
-  <si>
     <t>CORSIA</t>
   </si>
   <si>
-    <t>Una piantina √® una ... |Una ... avvolge una sigaretta |Una piantina avvolge una sigarettA</t>
-  </si>
-  <si>
     <t>CARTINA</t>
   </si>
   <si>
-    <t>Una coperta imbottita √® un ... |Un ... √® un giubbotto |Una coperta imbottita √® un giubbotto</t>
-  </si>
-  <si>
     <t>PIUMINO</t>
   </si>
   <si>
-    <t>Gli ecologisti lanciano un ... |Un ... √® una data d'esame |Gli ecologisti lanciano una data d'esame</t>
-  </si>
-  <si>
     <t>APPELLO</t>
   </si>
   <si>
-    <t>Arisa incide un ... |Un ... √® una raccolta di brani |Arisa incide una raccolta di brani</t>
-  </si>
-  <si>
     <t>ALBUM</t>
   </si>
   <si>
@@ -243,33 +197,18 @@
     <t>DIARIO</t>
   </si>
   <si>
-    <t>Una nave utilizza una ... |Una ... √® un molo del porto |Una nave utilizza un molo del porto</t>
-  </si>
-  <si>
     <t>BANCHINA</t>
   </si>
   <si>
-    <t>Un viaggiatore ha una ... |Una ... √® una carta geografica |Un viaggiatore ha una carta geografica</t>
-  </si>
-  <si>
     <t>MAPPA</t>
   </si>
   <si>
-    <t>Il giudice decreta il ... |Il ... √® una proroga |Il giudice decreta una proroga</t>
-  </si>
-  <si>
     <t>RINVIO</t>
   </si>
   <si>
-    <t>Il compositore scrive una ... |Una ... √® una composizione musicale |Il compositore scrive una composizione musicale</t>
-  </si>
-  <si>
     <t>MELODIA</t>
   </si>
   <si>
-    <t>Quella trasmissione √® una ... |Una ... contrasta il suo libro |Quella trasmissione contrasta il suo libro</t>
-  </si>
-  <si>
     <t>REPLICA</t>
   </si>
   <si>
@@ -309,198 +248,105 @@
     <t>DECOLLO</t>
   </si>
   <si>
-    <t>Il comico √® una ... |Una ... √® una linea di contorno |Il comico √® una linea di contorno</t>
-  </si>
-  <si>
     <t>SAGOMA</t>
   </si>
   <si>
-    <t>Mario segue il ... |Il ... √® un gruppo conformista |Mario segue un gruppo conformista</t>
-  </si>
-  <si>
     <t>GREGGE</t>
   </si>
   <si>
     <t>ARMATURA</t>
   </si>
   <si>
-    <t>Gigi guadagna la ... |La ... √® il sostentamento quotidiano |Gigi guadagna il sostentamento quotidiano</t>
-  </si>
-  <si>
     <t>PAGNOTTA</t>
   </si>
   <si>
     <t>REBUS</t>
   </si>
   <si>
-    <t>I valori costituiscono uno ... |Uno ... √® un sistema di riferimento |I valori costituiscono un sistema di riferimento</t>
-  </si>
-  <si>
     <t>SFONDO</t>
   </si>
   <si>
-    <t>L'amicizia √® un ... |Un ... √® un aiuto |L'amicizia √® un aiuto</t>
-  </si>
-  <si>
     <t>SUPPORTO</t>
   </si>
   <si>
-    <t>Franco ha chiuso un ... |Un ... √® una parte del libro |Franco ha chiuso una parte del libro</t>
-  </si>
-  <si>
     <t>CAPITOLO</t>
   </si>
   <si>
-    <t>Quella ragazza √® una ... |Una ... √® una pietra preziosa |Quella ragazza √® una pietra preziosa</t>
-  </si>
-  <si>
     <t>GEMMA</t>
   </si>
   <si>
-    <t>Uno tzunami √® un'... |Un'... √® una serie di eventi |Uno tzunami √® una serie di eventi</t>
-  </si>
-  <si>
     <t>ONDATA</t>
   </si>
   <si>
-    <t>La presidenza √® l‚Äô... |L‚Äô... √® la parte pi√π alta |La presidenza √® la parte pi√π alta</t>
-  </si>
-  <si>
     <t>APICE</t>
   </si>
   <si>
-    <t>Una risata √® un ... |Un ... serve alla salute |Una risata serve alla salute</t>
-  </si>
-  <si>
     <t>FARMACO</t>
   </si>
   <si>
-    <t>Il corpo √® un ... |Il ... √® sacro |Il corpo √® sacro</t>
-  </si>
-  <si>
     <t>TEMPIO</t>
   </si>
   <si>
     <t>V</t>
   </si>
   <si>
-    <t>Un vortice √® un ... |Un ... √® siciliano |Un vortice √® siciliano</t>
-  </si>
-  <si>
     <t>CANNOLO</t>
   </si>
   <si>
-    <t>Un'esperienza √® un ... |Un ... ha quattro ruote |Un'esperienza ha quattro ruote</t>
-  </si>
-  <si>
     <t>CAMPER</t>
   </si>
   <si>
-    <t>Una cozza √® un ... |Un ... contiene penne |Una cozza contiene penne</t>
-  </si>
-  <si>
     <t>ASTUCCIO</t>
   </si>
   <si>
-    <t>Il movimento √® una ... |Una ... ha una pagaia |Il movimento ha una pagaia</t>
-  </si>
-  <si>
     <t>CANOA</t>
   </si>
   <si>
-    <t>Il vento √® un ... |Un ... √® un uomo |Il vento √® un uomo</t>
-  </si>
-  <si>
     <t>BIDELLO</t>
   </si>
   <si>
-    <t>L‚ÄôAfrica √® un ... |Un ... decora le pareti |L‚ÄôAfrica decora le pareti</t>
-  </si>
-  <si>
     <t>ARAZZO</t>
   </si>
   <si>
-    <t>Il migliore amico √® un ... |Un ... √® una persona somigliante |Il migliore amico √® una persona somigliante</t>
-  </si>
-  <si>
     <t>SOSIA</t>
   </si>
   <si>
-    <t>L'altruismo √® una ... |Una ... √® uno slancio |L'altruismo √® uno slancio</t>
-  </si>
-  <si>
     <t>RINCORSA</t>
   </si>
   <si>
-    <t>La mafia √® un ... |Un ... ha tentacoli |La mafia ha tentacoli</t>
-  </si>
-  <si>
     <t>POLPO</t>
   </si>
   <si>
-    <t>Un fan √® uno ... |Uno ... favorisce l'organizzazione |Un fan favorisce l'organizzazione</t>
-  </si>
-  <si>
     <t>SPONSOR</t>
   </si>
   <si>
-    <t>L'odio √® una ... |Una ... √® arida |L'odio √® arido</t>
-  </si>
-  <si>
     <t>STEPPA</t>
   </si>
   <si>
-    <t>L'onore √® una ... |Una ... √® la difesa dell'identit√† |L'onore √® la difesa dell'identit√†</t>
-  </si>
-  <si>
     <t>CASATA</t>
   </si>
   <si>
-    <t>Il gallo √® un ... |Un ... √® un capo |Il gallo √® un capo</t>
-  </si>
-  <si>
     <t>FARAONE</t>
   </si>
   <si>
-    <t>Quel bimbo √® un ... |Il ... √® dolce |Quel bimbo √® dolce</t>
-  </si>
-  <si>
     <t>PANDORO</t>
   </si>
   <si>
-    <t>Un grido √® un ... |Un ... emette suoni |Un grido emette suoni</t>
-  </si>
-  <si>
     <t>MEGAFONO</t>
   </si>
   <si>
-    <t>Uno spirito √® uno ... |Uno ... √® un personaggio di fantasia |Uno spirito √® un personaggio di fantasia</t>
-  </si>
-  <si>
     <t>GNOMO</t>
   </si>
   <si>
-    <t>Il cuore √® un'... |Un'... trasporta liquidi |Il cuore trasporta liquidi</t>
-  </si>
-  <si>
     <t>ANFORA</t>
   </si>
   <si>
-    <t>Il lavoro √® un ... |Un ... serve nei campi |Il lavoro serve nei campi</t>
-  </si>
-  <si>
     <t>BADILE</t>
   </si>
   <si>
-    <t>La felpa ha il ... |il ... √® una bevanda |La felpa ha una bevanda</t>
-  </si>
-  <si>
     <t>CAPPUCCIO</t>
   </si>
   <si>
-    <t>Il Ticino √® un ... |Un ... √® un fiume |Il Ticino √® un fiume</t>
-  </si>
-  <si>
     <t>EMISSARIO</t>
   </si>
   <si>
@@ -510,75 +356,21 @@
     <t>CESTELLO</t>
   </si>
   <si>
-    <t>Sara gestisce una ... |Una ... √® un locale |Sara gestisce un locale</t>
-  </si>
-  <si>
     <t>DISCOTECA</t>
   </si>
   <si>
-    <t>Un punto fermo √® un ... |Un ... √® un piccolo palo |Un punto fermo √® un piccolo palo</t>
-  </si>
-  <si>
     <t>PALETTO</t>
   </si>
   <si>
-    <t>La laurea √® un ... |Un ... consente il riposo |La laurea consente il riposo</t>
-  </si>
-  <si>
     <t>APPRODO</t>
   </si>
   <si>
-    <t>La gioia √® una ... |Una ... √® vivace |La gioia √® vivace</t>
-  </si>
-  <si>
     <t>SAMBA</t>
   </si>
   <si>
-    <t>Il conforto √® una ... |Una ... Scende dalla nave |Il conforto scende dalla nave</t>
-  </si>
-  <si>
     <t>SCIALUPPA</t>
   </si>
   <si>
-    <t>La vita \xe8 un ... |Un ... √® complesso |La vita √® complessa</t>
-  </si>
-  <si>
-    <t>L'amicizia \xe8 un ... |Un ... √® una preparazione emolliente |L'amicizia √® una preparazione emolliente</t>
-  </si>
-  <si>
-    <t>Mario incide una ... |Una ... \xe8 un contenitore |Mario incide un contenitore</t>
-  </si>
-  <si>
-    <t>La benzina ha avuto un ... |Un ... \xe8 un rilievo |La benzina ha avuto un rilievo</t>
-  </si>
-  <si>
-    <t>Carla aggiunge una ... |Una ... \xe8 un piccolo involucro |Carla aggiunge un piccolo involucro</t>
-  </si>
-  <si>
-    <t>I soci fondatori sono il ... |Il ... \xe8 all'interno dell'atomo |I soci fondatori sono all'interno dell'atomo</t>
-  </si>
-  <si>
-    <t>Studiare \xe8 una ... |Una ... \xe8 una corsa podistica |Studiare √® una corsa podistica</t>
-  </si>
-  <si>
-    <t>L'occhio ha l'... |L'... \xe8 un insieme di colori |L'occhio ha un insieme di colori</t>
-  </si>
-  <si>
-    <t>L'attivit\xe0 ha visto un ... |Un ... \xe8 una manovra dell'aereo |L'attivit√† ha visto una manovra dell'aereo</t>
-  </si>
-  <si>
-    <t>La mamma \xe8 una ... |La ... cova le uova |La mamma cova le uova</t>
-  </si>
-  <si>
-    <t>L'aggressivit√† \xe8 un'... |Un'... √® una difesa |L'aggressivit√† √® una difesa</t>
-  </si>
-  <si>
-    <t>La prugna contiene il …</t>
-  </si>
-  <si>
-    <t>Il … è un albero</t>
-  </si>
-  <si>
     <t>La prugna contiene un albero</t>
   </si>
   <si>
@@ -589,6 +381,951 @@
   </si>
   <si>
     <t>conclusion</t>
+  </si>
+  <si>
+    <t>Fabrizio Corona è un ... |Un ... è un fiore |Fabrizio Corona è un fiore</t>
+  </si>
+  <si>
+    <t>I capelli hanno un ... |Un ... è un porcospino |I capelli hanno un porcospino</t>
+  </si>
+  <si>
+    <t>Un capitombolo è un ... |Un ... è un nastro arrotolato |Un capitombolo è un nastro arrotolato</t>
+  </si>
+  <si>
+    <t>La buccia è uno ... |Uno ... è una grossa differenza |La buccia è una grossa differenza</t>
+  </si>
+  <si>
+    <t>Il caseificio produce ... |... è formaggio |Il caseificio produce formaggio</t>
+  </si>
+  <si>
+    <t>La televisione è un ... |Un ... è molto diffuso |La televisione è molto diffusa</t>
+  </si>
+  <si>
+    <t>La zia coltiva il ... |Il ... è una pianta |La zia coltiva una pianta</t>
+  </si>
+  <si>
+    <t>Al bivio c'è un ... |Un ... è un'interruzione |Al bivio c'è un'interruzione</t>
+  </si>
+  <si>
+    <t>Belen è una ... |Una ... è una showgirl |Belen è una showgirl</t>
+  </si>
+  <si>
+    <t>Una scommessa è una ... |Una ... è trasmessa in TV |Una scommessa è trasmessa in TV</t>
+  </si>
+  <si>
+    <t>Un assortimento è una ... |Una ... è greca |Un assortimento è greco</t>
+  </si>
+  <si>
+    <t>Un portiere ha fatto una ... |Una ... è una sfilata militare |Un portiere ha fatto una sfilata militare</t>
+  </si>
+  <si>
+    <t>La guardia forestale ha una ... |Una ... è una somma illegale |La guardia forestale ha una somma illegale</t>
+  </si>
+  <si>
+    <t>A Verona c'è l'... |L'... è sabbia |A Verona c'è sabbia</t>
+  </si>
+  <si>
+    <t>Talete è un ... |Un ... è una lettura piacevole |Talete è una lettura piacevole</t>
+  </si>
+  <si>
+    <t>Un lingotto è una ... |Una ... è una lineetta |Un lingotto è una lineetta</t>
+  </si>
+  <si>
+    <t>La luna forma uno ... |Uno ... è una parte del frutto |La luna forma una parte del frutto</t>
+  </si>
+  <si>
+    <t>Il nuotatore percorre una ... |Una ... è una sezione stradale |Il nuotatore percorre una sezione stradale</t>
+  </si>
+  <si>
+    <t>Una piantina è una ... |Una ... avvolge una sigaretta |Una piantina avvolge una sigarettA</t>
+  </si>
+  <si>
+    <t>Una coperta imbottita è un ... |Un ... è un giubbotto |Una coperta imbottita è un giubbotto</t>
+  </si>
+  <si>
+    <t>Gli ecologisti lanciano un ... |Un ... è una data d'esame |Gli ecologisti lanciano una data d'esame</t>
+  </si>
+  <si>
+    <t>Arisa incide un ... |Un ... è una raccolta di brani |Arisa incide una raccolta di brani</t>
+  </si>
+  <si>
+    <t>Una nave utilizza una ... |Una ... è un molo del porto |Una nave utilizza un molo del porto</t>
+  </si>
+  <si>
+    <t>Un viaggiatore ha una ... |Una ... è una carta geografica |Un viaggiatore ha una carta geografica</t>
+  </si>
+  <si>
+    <t>Il giudice decreta il ... |Il ... è una proroga |Il giudice decreta una proroga</t>
+  </si>
+  <si>
+    <t>Il compositore scrive una ... |Una ... è una composizione musicale |Il compositore scrive una composizione musicale</t>
+  </si>
+  <si>
+    <t>Quella trasmissione è una ... |Una ... contrasta il suo libro |Quella trasmissione contrasta il suo libro</t>
+  </si>
+  <si>
+    <t>Il comico è una ... |Una ... è una linea di contorno |Il comico è una linea di contorno</t>
+  </si>
+  <si>
+    <t>Mario segue il ... |Il ... è un gruppo conformista |Mario segue un gruppo conformista</t>
+  </si>
+  <si>
+    <t>Gigi guadagna la ... |La ... è il sostentamento quotidiano |Gigi guadagna il sostentamento quotidiano</t>
+  </si>
+  <si>
+    <t>I valori costituiscono uno ... |Uno ... è un sistema di riferimento |I valori costituiscono un sistema di riferimento</t>
+  </si>
+  <si>
+    <t>L'amicizia è un ... |Un ... è un aiuto |L'amicizia è un aiuto</t>
+  </si>
+  <si>
+    <t>Franco ha chiuso un ... |Un ... è una parte del libro |Franco ha chiuso una parte del libro</t>
+  </si>
+  <si>
+    <t>Quella ragazza è una ... |Una ... è una pietra preziosa |Quella ragazza è una pietra preziosa</t>
+  </si>
+  <si>
+    <t>Uno tzunami è un'... |Un'... è una serie di eventi |Uno tzunami è una serie di eventi</t>
+  </si>
+  <si>
+    <t>Una risata è un ... |Un ... serve alla salute |Una risata serve alla salute</t>
+  </si>
+  <si>
+    <t>Il corpo è un ... |Il ... è sacro |Il corpo è sacro</t>
+  </si>
+  <si>
+    <t>Un vortice è un ... |Un ... è siciliano |Un vortice è siciliano</t>
+  </si>
+  <si>
+    <t>Un'esperienza è un ... |Un ... ha quattro ruote |Un'esperienza ha quattro ruote</t>
+  </si>
+  <si>
+    <t>Una cozza è un ... |Un ... contiene penne |Una cozza contiene penne</t>
+  </si>
+  <si>
+    <t>Il movimento è una ... |Una ... ha una pagaia |Il movimento ha una pagaia</t>
+  </si>
+  <si>
+    <t>Il vento è un ... |Un ... è un uomo |Il vento è un uomo</t>
+  </si>
+  <si>
+    <t>Il migliore amico è un ... |Un ... è una persona somigliante |Il migliore amico è una persona somigliante</t>
+  </si>
+  <si>
+    <t>L'altruismo è una ... |Una ... è uno slancio |L'altruismo è uno slancio</t>
+  </si>
+  <si>
+    <t>La mafia è un ... |Un ... ha tentacoli |La mafia ha tentacoli</t>
+  </si>
+  <si>
+    <t>Un fan è uno ... |Uno ... favorisce l'organizzazione |Un fan favorisce l'organizzazione</t>
+  </si>
+  <si>
+    <t>L'odio è una ... |Una ... è arida |L'odio è arido</t>
+  </si>
+  <si>
+    <t>Il gallo è un ... |Un ... è un capo |Il gallo è un capo</t>
+  </si>
+  <si>
+    <t>Quel bimbo è un ... |Il ... è dolce |Quel bimbo è dolce</t>
+  </si>
+  <si>
+    <t>Un grido è un ... |Un ... emette suoni |Un grido emette suoni</t>
+  </si>
+  <si>
+    <t>Uno spirito è uno ... |Uno ... è un personaggio di fantasia |Uno spirito è un personaggio di fantasia</t>
+  </si>
+  <si>
+    <t>Il cuore è un'... |Un'... trasporta liquidi |Il cuore trasporta liquidi</t>
+  </si>
+  <si>
+    <t>Il lavoro è un ... |Un ... serve nei campi |Il lavoro serve nei campi</t>
+  </si>
+  <si>
+    <t>La felpa ha il ... |il ... è una bevanda |La felpa ha una bevanda</t>
+  </si>
+  <si>
+    <t>Il Ticino è un ... |Un ... è un fiume |Il Ticino è un fiume</t>
+  </si>
+  <si>
+    <t>Sara gestisce una ... |Una ... è un locale |Sara gestisce un locale</t>
+  </si>
+  <si>
+    <t>Un punto fermo è un ... |Un ... è un piccolo palo |Un punto fermo è un piccolo palo</t>
+  </si>
+  <si>
+    <t>La laurea è un ... |Un ... consente il riposo |La laurea consente il riposo</t>
+  </si>
+  <si>
+    <t>La gioia è una ... |Una ... è vivace |La gioia è vivace</t>
+  </si>
+  <si>
+    <t>Il conforto è una ... |Una ... Scende dalla nave |Il conforto scende dalla nave</t>
+  </si>
+  <si>
+    <t>La presidenza è l'... |L'... è la parte pi√π alta |La presidenza è la parte pi√π alta</t>
+  </si>
+  <si>
+    <t>L'Africa è un ... |Un ... decora le pareti |L'Africa decora le pareti</t>
+  </si>
+  <si>
+    <t>In montagna c'è una ... |Una ... è un piano inclinato |In montagna c'è un piano inclinato</t>
+  </si>
+  <si>
+    <t>La prugna contiene il ... |Il ... è un albero |La prugna contiene un albero</t>
+  </si>
+  <si>
+    <t>L'onore è una ... |Una ... è la difesa dell'identità |L'onore è la difesa dell'identità</t>
+  </si>
+  <si>
+    <t>Una certa quantità è un ... |Un ... scava buche |Una certa quantità scava buche</t>
+  </si>
+  <si>
+    <t>La vita è un ... |Un ... è complesso |La vita è complessa</t>
+  </si>
+  <si>
+    <t>Mario incide una ... |Una ... è un contenitore |Mario incide un contenitore</t>
+  </si>
+  <si>
+    <t>L'occhio ha l'... |L'... è un insieme di colori |L'occhio ha un insieme di colori</t>
+  </si>
+  <si>
+    <t>La benzina ha avuto un ... |Un ... è un rilievo |La benzina ha avuto un rilievo</t>
+  </si>
+  <si>
+    <t>Carla aggiunge una ... |Una ... è un piccolo involucro |Carla aggiunge un piccolo involucro</t>
+  </si>
+  <si>
+    <t>Studiare è una ... |Una ... è una corsa podistica |Studiare è una corsa podistica</t>
+  </si>
+  <si>
+    <t>La mamma è una ... |La ... cova le uova |La mamma cova le uova</t>
+  </si>
+  <si>
+    <t>I soci fondatori sono il ... |Il ... è all'interno dell'atomo |I soci fondatori sono all'interno dell'atomo</t>
+  </si>
+  <si>
+    <t>L'amicizia è un ... |Un ... è una preparazione emolliente |L'amicizia è una preparazione emolliente</t>
+  </si>
+  <si>
+    <t>L'attivit\xe0 ha visto un ... |Un ... è una manovra dell'aereo |L'attività ha visto una manovra dell'aereo</t>
+  </si>
+  <si>
+    <t>L'aggressività è un'... |Un'... è una difesa |L'aggressività è una difesa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... scava buche </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I capelli hanno un ... </t>
+  </si>
+  <si>
+    <t>I capelli hanno un porcospino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il caseificio produce ... </t>
+  </si>
+  <si>
+    <t>Il caseificio produce formaggio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La zia coltiva il ... </t>
+  </si>
+  <si>
+    <t>La zia coltiva una pianta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un portiere ha fatto una ... </t>
+  </si>
+  <si>
+    <t>Un portiere ha fatto una sfilata militare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La guardia forestale ha una ... </t>
+  </si>
+  <si>
+    <t>La guardia forestale ha una somma illegale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La luna forma uno ... </t>
+  </si>
+  <si>
+    <t>La luna forma una parte del frutto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il nuotatore percorre una ... </t>
+  </si>
+  <si>
+    <t>Il nuotatore percorre una sezione stradale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... avvolge una sigaretta </t>
+  </si>
+  <si>
+    <t>Una piantina avvolge una sigarettA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gli ecologisti lanciano un ... </t>
+  </si>
+  <si>
+    <t>Gli ecologisti lanciano una data d'esame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arisa incide un ... </t>
+  </si>
+  <si>
+    <t>Arisa incide una raccolta di brani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anna Frank ha scritto un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... contiene pensieri </t>
+  </si>
+  <si>
+    <t>Anna Frank ha scritto pensieri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una nave utilizza una ... </t>
+  </si>
+  <si>
+    <t>Una nave utilizza un molo del porto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un viaggiatore ha una ... </t>
+  </si>
+  <si>
+    <t>Un viaggiatore ha una carta geografica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il giudice decreta il ... </t>
+  </si>
+  <si>
+    <t>Il giudice decreta una proroga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il compositore scrive una ... </t>
+  </si>
+  <si>
+    <t>Il compositore scrive una composizione musicale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... contrasta il suo libro </t>
+  </si>
+  <si>
+    <t>Quella trasmissione contrasta il suo libro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mario incide una ... </t>
+  </si>
+  <si>
+    <t>Mario incide un contenitore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'occhio ha l'... </t>
+  </si>
+  <si>
+    <t>L'occhio ha un insieme di colori</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La benzina ha avuto un ... </t>
+  </si>
+  <si>
+    <t>La benzina ha avuto un rilievo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carla aggiunge una ... </t>
+  </si>
+  <si>
+    <t>Carla aggiunge un piccolo involucro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il papa ha un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... ha un elettorato </t>
+  </si>
+  <si>
+    <t>Il papa ha un elettorato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La ... cova le uova </t>
+  </si>
+  <si>
+    <t>La mamma cova le uova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I soci fondatori sono il ... </t>
+  </si>
+  <si>
+    <t>I soci fondatori sono all'interno dell'atomo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mario segue il ... </t>
+  </si>
+  <si>
+    <t>Mario segue un gruppo conformista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gigi guadagna la ... </t>
+  </si>
+  <si>
+    <t>Gigi guadagna il sostentamento quotidiano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I valori costituiscono uno ... </t>
+  </si>
+  <si>
+    <t>I valori costituiscono un sistema di riferimento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Franco ha chiuso un ... </t>
+  </si>
+  <si>
+    <t>Franco ha chiuso una parte del libro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... serve alla salute </t>
+  </si>
+  <si>
+    <t>Una risata serve alla salute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... ha quattro ruote </t>
+  </si>
+  <si>
+    <t>Un'esperienza ha quattro ruote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... contiene penne </t>
+  </si>
+  <si>
+    <t>Una cozza contiene penne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... ha una pagaia </t>
+  </si>
+  <si>
+    <t>Il movimento ha una pagaia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... decora le pareti </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... ha tentacoli </t>
+  </si>
+  <si>
+    <t>La mafia ha tentacoli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uno ... favorisce l'organizzazione </t>
+  </si>
+  <si>
+    <t>Un fan favorisce l'organizzazione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... emette suoni </t>
+  </si>
+  <si>
+    <t>Un grido emette suoni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un'... trasporta liquidi </t>
+  </si>
+  <si>
+    <t>Il cuore trasporta liquidi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... serve nei campi </t>
+  </si>
+  <si>
+    <t>Il lavoro serve nei campi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La felpa ha il ... </t>
+  </si>
+  <si>
+    <t>La felpa ha una bevanda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La lavatrice ha un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... contiene bottiglie </t>
+  </si>
+  <si>
+    <t>La lavatrice contiene bottiglie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sara gestisce una ... </t>
+  </si>
+  <si>
+    <t>Sara gestisce un locale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... consente il riposo </t>
+  </si>
+  <si>
+    <t>La laurea consente il riposo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... Scende dalla nave </t>
+  </si>
+  <si>
+    <t>Il conforto scende dalla nave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il ... è un albero </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fabrizio Corona è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è un fiore </t>
+  </si>
+  <si>
+    <t>Fabrizio Corona è un fiore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La prugna contiene il … </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una certa quantità è un ... </t>
+  </si>
+  <si>
+    <t>Una certa quantità scava buche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è un porcospino </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un capitombolo è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è un nastro arrotolato </t>
+  </si>
+  <si>
+    <t>Un capitombolo è un nastro arrotolato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La buccia è uno ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uno ... è una grossa differenza </t>
+  </si>
+  <si>
+    <t>La buccia è una grossa differenza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">... è formaggio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La televisione è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è molto diffuso </t>
+  </si>
+  <si>
+    <t>La televisione è molto diffusa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il ... è una pianta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al bivio c'è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è un'interruzione </t>
+  </si>
+  <si>
+    <t>Al bivio c'è un'interruzione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belen è una ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è una showgirl </t>
+  </si>
+  <si>
+    <t>Belen è una showgirl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In montagna c’è una ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è un piano inclinato </t>
+  </si>
+  <si>
+    <t>In montagna c’è un piano inclinato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una scommessa è una ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è trasmessa in TV </t>
+  </si>
+  <si>
+    <t>Una scommessa è trasmessa in TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un assortimento è una ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è greca </t>
+  </si>
+  <si>
+    <t>Un assortimento è greco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è una sfilata militare </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è una somma illegale </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Verona c'è l'... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'... è sabbia </t>
+  </si>
+  <si>
+    <t>A Verona c'è sabbia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talete è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è una lettura piacevole </t>
+  </si>
+  <si>
+    <t>Talete è una lettura piacevole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un lingotto è una ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è una lineetta </t>
+  </si>
+  <si>
+    <t>Un lingotto è una lineetta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uno ... è una parte del frutto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è una sezione stradale </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una piantina è una ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una coperta imbottita è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è un giubbotto </t>
+  </si>
+  <si>
+    <t>Una coperta imbottita è un giubbotto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è una data d'esame </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è una raccolta di brani </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è un molo del porto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è una carta geografica </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il ... è una proroga </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è una composizione musicale </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quella trasmissione è una ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è un contenitore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'... è un insieme di colori </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è un rilievo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è un piccolo involucro </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Studiare è una ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è una corsa podistica </t>
+  </si>
+  <si>
+    <t>Studiare è una corsa podistica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La mamma è una ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il ... è all'interno dell'atomo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'amicizia è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è una preparazione emolliente </t>
+  </si>
+  <si>
+    <t>L'amicizia è una preparazione emolliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'attività ha visto un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è una manovra dell'aereo </t>
+  </si>
+  <si>
+    <t>L'attività ha visto una manovra dell'aereo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il comico è una ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è una linea di contorno </t>
+  </si>
+  <si>
+    <t>Il comico è una linea di contorno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il ... è un gruppo conformista </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'aggressività è un'... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un'... è una difesa </t>
+  </si>
+  <si>
+    <t>L'aggressività è una difesa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La ... è il sostentamento quotidiano </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La vita è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è complesso </t>
+  </si>
+  <si>
+    <t>La vita è complessa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uno ... è un sistema di riferimento </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è un aiuto </t>
+  </si>
+  <si>
+    <t>L'amicizia è un aiuto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è una parte del libro </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quella ragazza è una ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è una pietra preziosa </t>
+  </si>
+  <si>
+    <t>Quella ragazza è una pietra preziosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uno tzunami è un'... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un'... è una serie di eventi </t>
+  </si>
+  <si>
+    <t>Uno tzunami è una serie di eventi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La presidenza è l’... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’... è la parte più alta </t>
+  </si>
+  <si>
+    <t>La presidenza è la parte più alta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una risata è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il corpo è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il ... è sacro </t>
+  </si>
+  <si>
+    <t>Il corpo è sacro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un vortice è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è siciliano </t>
+  </si>
+  <si>
+    <t>Un vortice è siciliano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un'esperienza è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una cozza è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il movimento è una ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il vento è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è un uomo </t>
+  </si>
+  <si>
+    <t>Il vento è un uomo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’Africa è un ... </t>
+  </si>
+  <si>
+    <t>L’Africa decora le pareti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il migliore amico è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è una persona somigliante </t>
+  </si>
+  <si>
+    <t>Il migliore amico è una persona somigliante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'altruismo è una ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è uno slancio </t>
+  </si>
+  <si>
+    <t>L'altruismo è uno slancio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La mafia è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un fan è uno ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'odio è una ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è arida </t>
+  </si>
+  <si>
+    <t>L'odio è arido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'onore è una ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è la difesa dell'identità </t>
+  </si>
+  <si>
+    <t>L'onore è la difesa dell'identità</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il gallo è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è un capo </t>
+  </si>
+  <si>
+    <t>Il gallo è un capo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quel bimbo è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il ... è dolce </t>
+  </si>
+  <si>
+    <t>Quel bimbo è dolce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un grido è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uno spirito è uno ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uno ... è un personaggio di fantasia </t>
+  </si>
+  <si>
+    <t>Uno spirito è un personaggio di fantasia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il cuore è un'... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il lavoro è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">il ... è una bevanda </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il Ticino è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è un fiume </t>
+  </si>
+  <si>
+    <t>Il Ticino è un fiume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è un locale </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un punto fermo è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un ... è un piccolo palo </t>
+  </si>
+  <si>
+    <t>Un punto fermo è un piccolo palo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La laurea è un ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La gioia è una ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una ... è vivace </t>
+  </si>
+  <si>
+    <t>La gioia è vivace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il conforto è una ... </t>
   </si>
 </sst>
 </file>
@@ -637,8 +1374,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -647,11 +1390,17 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -660,7 +1409,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="arguments" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="arguments" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="arg copy 2" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -987,8 +1740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -997,8 +1750,8 @@
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="29.33203125" customWidth="1"/>
+    <col min="6" max="6" width="49.1640625" customWidth="1"/>
+    <col min="7" max="7" width="35.33203125" customWidth="1"/>
     <col min="8" max="8" width="29.6640625" customWidth="1"/>
     <col min="9" max="9" width="37.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
@@ -1024,13 +1777,13 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>180</v>
+        <v>101</v>
       </c>
       <c r="H1" t="s">
-        <v>181</v>
+        <v>102</v>
       </c>
       <c r="I1" t="s">
-        <v>182</v>
+        <v>103</v>
       </c>
       <c r="J1" t="s">
         <v>6</v>
@@ -1053,19 +1806,19 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G2" t="s">
+        <v>272</v>
+      </c>
+      <c r="H2" t="s">
+        <v>268</v>
+      </c>
+      <c r="I2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J2" t="s">
         <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>177</v>
-      </c>
-      <c r="H2" t="s">
-        <v>178</v>
-      </c>
-      <c r="I2" t="s">
-        <v>179</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1085,19 +1838,19 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>169</v>
       </c>
       <c r="G3" t="s">
-        <v>177</v>
+        <v>273</v>
       </c>
       <c r="H3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="I3" t="s">
-        <v>179</v>
+        <v>274</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1117,19 +1870,19 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>104</v>
       </c>
       <c r="G4" t="s">
-        <v>177</v>
+        <v>269</v>
       </c>
       <c r="H4" t="s">
-        <v>178</v>
+        <v>270</v>
       </c>
       <c r="I4" t="s">
-        <v>179</v>
+        <v>271</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1149,19 +1902,19 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="G5" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="H5" t="s">
-        <v>178</v>
+        <v>275</v>
       </c>
       <c r="I5" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="J5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1181,19 +1934,19 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="G6" t="s">
-        <v>177</v>
+        <v>276</v>
       </c>
       <c r="H6" t="s">
-        <v>178</v>
+        <v>277</v>
       </c>
       <c r="I6" t="s">
-        <v>179</v>
+        <v>278</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1213,19 +1966,19 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>107</v>
       </c>
       <c r="G7" t="s">
-        <v>177</v>
+        <v>279</v>
       </c>
       <c r="H7" t="s">
-        <v>178</v>
+        <v>280</v>
       </c>
       <c r="I7" t="s">
-        <v>179</v>
+        <v>281</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1239,25 +1992,25 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>108</v>
       </c>
       <c r="G8" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="H8" t="s">
-        <v>178</v>
+        <v>282</v>
       </c>
       <c r="I8" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="J8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1271,25 +2024,25 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="G9" t="s">
-        <v>177</v>
+        <v>283</v>
       </c>
       <c r="H9" t="s">
-        <v>178</v>
+        <v>284</v>
       </c>
       <c r="I9" t="s">
-        <v>179</v>
+        <v>285</v>
       </c>
       <c r="J9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1303,25 +2056,25 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>110</v>
       </c>
       <c r="G10" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="H10" t="s">
-        <v>178</v>
+        <v>286</v>
       </c>
       <c r="I10" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="J10" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1335,25 +2088,25 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="G11" t="s">
-        <v>177</v>
+        <v>287</v>
       </c>
       <c r="H11" t="s">
-        <v>178</v>
+        <v>288</v>
       </c>
       <c r="I11" t="s">
-        <v>179</v>
+        <v>289</v>
       </c>
       <c r="J11" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1367,25 +2120,25 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>112</v>
+      </c>
+      <c r="G12" t="s">
+        <v>290</v>
+      </c>
+      <c r="H12" t="s">
+        <v>291</v>
+      </c>
+      <c r="I12" t="s">
+        <v>292</v>
+      </c>
+      <c r="J12" t="s">
         <v>23</v>
-      </c>
-      <c r="E12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" t="s">
-        <v>177</v>
-      </c>
-      <c r="H12" t="s">
-        <v>178</v>
-      </c>
-      <c r="I12" t="s">
-        <v>179</v>
-      </c>
-      <c r="J12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1399,25 +2152,25 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>166</v>
+      </c>
+      <c r="G13" t="s">
+        <v>293</v>
+      </c>
+      <c r="H13" t="s">
+        <v>294</v>
+      </c>
+      <c r="I13" t="s">
+        <v>295</v>
+      </c>
+      <c r="J13" t="s">
         <v>24</v>
-      </c>
-      <c r="F13" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" t="s">
-        <v>177</v>
-      </c>
-      <c r="H13" t="s">
-        <v>178</v>
-      </c>
-      <c r="I13" t="s">
-        <v>179</v>
-      </c>
-      <c r="J13" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1431,25 +2184,25 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="G14" t="s">
-        <v>177</v>
+        <v>296</v>
       </c>
       <c r="H14" t="s">
-        <v>178</v>
+        <v>297</v>
       </c>
       <c r="I14" t="s">
-        <v>179</v>
+        <v>298</v>
       </c>
       <c r="J14" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1463,25 +2216,25 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="G15" t="s">
-        <v>177</v>
+        <v>299</v>
       </c>
       <c r="H15" t="s">
-        <v>178</v>
+        <v>300</v>
       </c>
       <c r="I15" t="s">
-        <v>179</v>
+        <v>301</v>
       </c>
       <c r="J15" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1495,25 +2248,25 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>42</v>
+        <v>115</v>
       </c>
       <c r="G16" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="H16" t="s">
-        <v>178</v>
+        <v>302</v>
       </c>
       <c r="I16" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="J16" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1527,25 +2280,25 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>44</v>
+        <v>116</v>
       </c>
       <c r="G17" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="H17" t="s">
-        <v>178</v>
+        <v>303</v>
       </c>
       <c r="I17" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="J17" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1559,25 +2312,25 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="G18" t="s">
-        <v>177</v>
+        <v>304</v>
       </c>
       <c r="H18" t="s">
-        <v>178</v>
+        <v>305</v>
       </c>
       <c r="I18" t="s">
-        <v>179</v>
+        <v>306</v>
       </c>
       <c r="J18" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1591,25 +2344,25 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
+        <v>118</v>
       </c>
       <c r="G19" t="s">
-        <v>177</v>
+        <v>307</v>
       </c>
       <c r="H19" t="s">
-        <v>178</v>
+        <v>308</v>
       </c>
       <c r="I19" t="s">
-        <v>179</v>
+        <v>309</v>
       </c>
       <c r="J19" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1617,7 +2370,7 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1629,19 +2382,19 @@
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="G20" t="s">
-        <v>177</v>
+        <v>310</v>
       </c>
       <c r="H20" t="s">
-        <v>178</v>
+        <v>311</v>
       </c>
       <c r="I20" t="s">
-        <v>179</v>
+        <v>312</v>
       </c>
       <c r="J20" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1649,7 +2402,7 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1661,19 +2414,19 @@
         <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>53</v>
+        <v>120</v>
       </c>
       <c r="G21" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="H21" t="s">
-        <v>178</v>
+        <v>313</v>
       </c>
       <c r="I21" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="J21" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1681,7 +2434,7 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -1693,19 +2446,19 @@
         <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>55</v>
+        <v>121</v>
       </c>
       <c r="G22" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="H22" t="s">
-        <v>178</v>
+        <v>314</v>
       </c>
       <c r="I22" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="J22" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1713,7 +2466,7 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C23">
         <v>4</v>
@@ -1725,19 +2478,19 @@
         <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>57</v>
+        <v>122</v>
       </c>
       <c r="G23" t="s">
-        <v>177</v>
+        <v>315</v>
       </c>
       <c r="H23" t="s">
-        <v>178</v>
+        <v>196</v>
       </c>
       <c r="I23" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="J23" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1745,7 +2498,7 @@
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -1757,19 +2510,19 @@
         <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="G24" t="s">
-        <v>177</v>
+        <v>316</v>
       </c>
       <c r="H24" t="s">
-        <v>178</v>
+        <v>317</v>
       </c>
       <c r="I24" t="s">
-        <v>179</v>
+        <v>318</v>
       </c>
       <c r="J24" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1777,7 +2530,7 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C25">
         <v>6</v>
@@ -1789,19 +2542,19 @@
         <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="G25" t="s">
-        <v>177</v>
+        <v>198</v>
       </c>
       <c r="H25" t="s">
-        <v>178</v>
+        <v>319</v>
       </c>
       <c r="I25" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="J25" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1809,31 +2562,31 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C26">
         <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F26" t="s">
-        <v>63</v>
+        <v>125</v>
       </c>
       <c r="G26" t="s">
-        <v>177</v>
+        <v>200</v>
       </c>
       <c r="H26" t="s">
-        <v>178</v>
+        <v>320</v>
       </c>
       <c r="I26" t="s">
-        <v>179</v>
+        <v>201</v>
       </c>
       <c r="J26" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1841,31 +2594,31 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C27">
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E27" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F27" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="G27" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="H27" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="I27" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="J27" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1873,31 +2626,31 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C28">
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F28" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="G28" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
       <c r="H28" t="s">
-        <v>178</v>
+        <v>321</v>
       </c>
       <c r="I28" t="s">
-        <v>179</v>
+        <v>206</v>
       </c>
       <c r="J28" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1905,31 +2658,31 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C29">
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F29" t="s">
-        <v>69</v>
+        <v>127</v>
       </c>
       <c r="G29" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
       <c r="H29" t="s">
-        <v>178</v>
+        <v>322</v>
       </c>
       <c r="I29" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
       <c r="J29" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1937,31 +2690,31 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C30">
         <v>11</v>
       </c>
       <c r="D30" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F30" t="s">
-        <v>71</v>
+        <v>128</v>
       </c>
       <c r="G30" t="s">
-        <v>177</v>
+        <v>209</v>
       </c>
       <c r="H30" t="s">
-        <v>178</v>
+        <v>323</v>
       </c>
       <c r="I30" t="s">
-        <v>179</v>
+        <v>210</v>
       </c>
       <c r="J30" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1969,31 +2722,31 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C31">
         <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F31" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="G31" t="s">
-        <v>177</v>
+        <v>211</v>
       </c>
       <c r="H31" t="s">
-        <v>178</v>
+        <v>324</v>
       </c>
       <c r="I31" t="s">
-        <v>179</v>
+        <v>212</v>
       </c>
       <c r="J31" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2001,31 +2754,31 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C32">
         <v>13</v>
       </c>
       <c r="D32" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="G32" t="s">
-        <v>177</v>
+        <v>325</v>
       </c>
       <c r="H32" t="s">
-        <v>178</v>
+        <v>213</v>
       </c>
       <c r="I32" t="s">
-        <v>179</v>
+        <v>214</v>
       </c>
       <c r="J32" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2033,31 +2786,31 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C33">
         <v>14</v>
       </c>
       <c r="D33" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
       </c>
       <c r="F33" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="G33" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="H33" t="s">
-        <v>178</v>
+        <v>326</v>
       </c>
       <c r="I33" t="s">
-        <v>179</v>
+        <v>216</v>
       </c>
       <c r="J33" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2065,31 +2818,31 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C34">
         <v>15</v>
       </c>
       <c r="D34" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G34" t="s">
-        <v>177</v>
+        <v>217</v>
       </c>
       <c r="H34" t="s">
-        <v>178</v>
+        <v>327</v>
       </c>
       <c r="I34" t="s">
-        <v>179</v>
+        <v>218</v>
       </c>
       <c r="J34" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -2097,31 +2850,31 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C35">
         <v>16</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
       </c>
       <c r="F35" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="G35" t="s">
-        <v>177</v>
+        <v>219</v>
       </c>
       <c r="H35" t="s">
-        <v>178</v>
+        <v>328</v>
       </c>
       <c r="I35" t="s">
-        <v>179</v>
+        <v>220</v>
       </c>
       <c r="J35" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2129,31 +2882,31 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C36">
         <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
       </c>
       <c r="F36" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G36" t="s">
-        <v>177</v>
+        <v>221</v>
       </c>
       <c r="H36" t="s">
-        <v>178</v>
+        <v>329</v>
       </c>
       <c r="I36" t="s">
-        <v>179</v>
+        <v>222</v>
       </c>
       <c r="J36" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2161,31 +2914,31 @@
         <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C37">
         <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
       </c>
       <c r="F37" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="G37" t="s">
-        <v>177</v>
+        <v>223</v>
       </c>
       <c r="H37" t="s">
-        <v>178</v>
+        <v>224</v>
       </c>
       <c r="I37" t="s">
-        <v>179</v>
+        <v>225</v>
       </c>
       <c r="J37" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2193,7 +2946,7 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2205,19 +2958,19 @@
         <v>10</v>
       </c>
       <c r="F38" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="G38" t="s">
-        <v>177</v>
+        <v>330</v>
       </c>
       <c r="H38" t="s">
-        <v>178</v>
+        <v>331</v>
       </c>
       <c r="I38" t="s">
-        <v>179</v>
+        <v>332</v>
       </c>
       <c r="J38" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2225,7 +2978,7 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C39">
         <v>2</v>
@@ -2237,19 +2990,19 @@
         <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G39" t="s">
-        <v>177</v>
+        <v>333</v>
       </c>
       <c r="H39" t="s">
-        <v>178</v>
+        <v>226</v>
       </c>
       <c r="I39" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="J39" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2257,7 +3010,7 @@
         <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C40">
         <v>3</v>
@@ -2269,19 +3022,19 @@
         <v>10</v>
       </c>
       <c r="F40" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="G40" t="s">
-        <v>177</v>
+        <v>228</v>
       </c>
       <c r="H40" t="s">
-        <v>178</v>
+        <v>334</v>
       </c>
       <c r="I40" t="s">
-        <v>179</v>
+        <v>229</v>
       </c>
       <c r="J40" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2289,7 +3042,7 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C41">
         <v>4</v>
@@ -2301,19 +3054,19 @@
         <v>10</v>
       </c>
       <c r="F41" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="G41" t="s">
-        <v>177</v>
+        <v>335</v>
       </c>
       <c r="H41" t="s">
-        <v>178</v>
+        <v>336</v>
       </c>
       <c r="I41" t="s">
-        <v>179</v>
+        <v>337</v>
       </c>
       <c r="J41" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2321,7 +3074,7 @@
         <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C42">
         <v>5</v>
@@ -2333,19 +3086,19 @@
         <v>10</v>
       </c>
       <c r="F42" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="G42" t="s">
-        <v>177</v>
+        <v>338</v>
       </c>
       <c r="H42" t="s">
-        <v>178</v>
+        <v>339</v>
       </c>
       <c r="I42" t="s">
-        <v>179</v>
+        <v>340</v>
       </c>
       <c r="J42" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2353,7 +3106,7 @@
         <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C43">
         <v>6</v>
@@ -2365,19 +3118,19 @@
         <v>10</v>
       </c>
       <c r="F43" t="s">
-        <v>89</v>
+        <v>131</v>
       </c>
       <c r="G43" t="s">
-        <v>177</v>
+        <v>341</v>
       </c>
       <c r="H43" t="s">
-        <v>178</v>
+        <v>342</v>
       </c>
       <c r="I43" t="s">
-        <v>179</v>
+        <v>343</v>
       </c>
       <c r="J43" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2385,31 +3138,31 @@
         <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C44">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F44" t="s">
-        <v>91</v>
+        <v>132</v>
       </c>
       <c r="G44" t="s">
-        <v>177</v>
+        <v>230</v>
       </c>
       <c r="H44" t="s">
-        <v>178</v>
+        <v>344</v>
       </c>
       <c r="I44" t="s">
-        <v>179</v>
+        <v>231</v>
       </c>
       <c r="J44" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2417,31 +3170,31 @@
         <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C45">
         <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F45" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="G45" t="s">
-        <v>177</v>
+        <v>345</v>
       </c>
       <c r="H45" t="s">
-        <v>178</v>
+        <v>346</v>
       </c>
       <c r="I45" t="s">
-        <v>179</v>
+        <v>347</v>
       </c>
       <c r="J45" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2449,31 +3202,31 @@
         <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C46">
         <v>9</v>
       </c>
       <c r="D46" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E46" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F46" t="s">
-        <v>94</v>
+        <v>133</v>
       </c>
       <c r="G46" t="s">
-        <v>177</v>
+        <v>232</v>
       </c>
       <c r="H46" t="s">
-        <v>178</v>
+        <v>348</v>
       </c>
       <c r="I46" t="s">
-        <v>179</v>
+        <v>233</v>
       </c>
       <c r="J46" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2481,31 +3234,31 @@
         <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C47">
         <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F47" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="G47" t="s">
-        <v>177</v>
+        <v>349</v>
       </c>
       <c r="H47" t="s">
-        <v>178</v>
+        <v>350</v>
       </c>
       <c r="I47" t="s">
-        <v>179</v>
+        <v>351</v>
       </c>
       <c r="J47" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2513,31 +3266,31 @@
         <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C48">
         <v>11</v>
       </c>
       <c r="D48" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E48" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F48" t="s">
-        <v>97</v>
+        <v>134</v>
       </c>
       <c r="G48" t="s">
-        <v>177</v>
+        <v>234</v>
       </c>
       <c r="H48" t="s">
-        <v>178</v>
+        <v>352</v>
       </c>
       <c r="I48" t="s">
-        <v>179</v>
+        <v>235</v>
       </c>
       <c r="J48" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2545,31 +3298,31 @@
         <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C49">
         <v>12</v>
       </c>
       <c r="D49" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E49" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F49" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
       <c r="G49" t="s">
-        <v>177</v>
+        <v>335</v>
       </c>
       <c r="H49" t="s">
-        <v>178</v>
+        <v>353</v>
       </c>
       <c r="I49" t="s">
-        <v>179</v>
+        <v>354</v>
       </c>
       <c r="J49" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2577,31 +3330,31 @@
         <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C50">
         <v>13</v>
       </c>
       <c r="D50" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E50" t="s">
         <v>10</v>
       </c>
       <c r="F50" t="s">
-        <v>101</v>
+        <v>136</v>
       </c>
       <c r="G50" t="s">
-        <v>177</v>
+        <v>236</v>
       </c>
       <c r="H50" t="s">
-        <v>178</v>
+        <v>355</v>
       </c>
       <c r="I50" t="s">
-        <v>179</v>
+        <v>237</v>
       </c>
       <c r="J50" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2609,31 +3362,31 @@
         <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C51">
         <v>14</v>
       </c>
       <c r="D51" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E51" t="s">
         <v>10</v>
       </c>
       <c r="F51" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="G51" t="s">
-        <v>177</v>
+        <v>356</v>
       </c>
       <c r="H51" t="s">
-        <v>178</v>
+        <v>357</v>
       </c>
       <c r="I51" t="s">
-        <v>179</v>
+        <v>358</v>
       </c>
       <c r="J51" t="s">
-        <v>104</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2641,31 +3394,31 @@
         <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C52">
         <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E52" t="s">
         <v>10</v>
       </c>
       <c r="F52" t="s">
-        <v>105</v>
+        <v>138</v>
       </c>
       <c r="G52" t="s">
-        <v>177</v>
+        <v>359</v>
       </c>
       <c r="H52" t="s">
-        <v>178</v>
+        <v>360</v>
       </c>
       <c r="I52" t="s">
-        <v>179</v>
+        <v>361</v>
       </c>
       <c r="J52" t="s">
-        <v>106</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2673,31 +3426,31 @@
         <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C53">
         <v>16</v>
       </c>
       <c r="D53" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E53" t="s">
         <v>10</v>
       </c>
       <c r="F53" t="s">
-        <v>107</v>
+        <v>164</v>
       </c>
       <c r="G53" t="s">
-        <v>177</v>
+        <v>362</v>
       </c>
       <c r="H53" t="s">
-        <v>178</v>
+        <v>363</v>
       </c>
       <c r="I53" t="s">
-        <v>179</v>
+        <v>364</v>
       </c>
       <c r="J53" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2705,31 +3458,31 @@
         <v>7</v>
       </c>
       <c r="B54" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C54">
         <v>17</v>
       </c>
       <c r="D54" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E54" t="s">
         <v>10</v>
       </c>
       <c r="F54" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="G54" t="s">
-        <v>177</v>
+        <v>365</v>
       </c>
       <c r="H54" t="s">
-        <v>178</v>
+        <v>238</v>
       </c>
       <c r="I54" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
       <c r="J54" t="s">
-        <v>110</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2737,31 +3490,31 @@
         <v>7</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C55">
         <v>18</v>
       </c>
       <c r="D55" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E55" t="s">
         <v>10</v>
       </c>
       <c r="F55" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="G55" t="s">
-        <v>177</v>
+        <v>366</v>
       </c>
       <c r="H55" t="s">
-        <v>178</v>
+        <v>367</v>
       </c>
       <c r="I55" t="s">
-        <v>179</v>
+        <v>368</v>
       </c>
       <c r="J55" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2769,7 +3522,7 @@
         <v>7</v>
       </c>
       <c r="B56" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -2781,19 +3534,19 @@
         <v>10</v>
       </c>
       <c r="F56" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="G56" t="s">
-        <v>177</v>
+        <v>369</v>
       </c>
       <c r="H56" t="s">
-        <v>178</v>
+        <v>370</v>
       </c>
       <c r="I56" t="s">
-        <v>179</v>
+        <v>371</v>
       </c>
       <c r="J56" t="s">
-        <v>115</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2801,7 +3554,7 @@
         <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C57">
         <v>2</v>
@@ -2813,19 +3566,19 @@
         <v>10</v>
       </c>
       <c r="F57" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="G57" t="s">
-        <v>177</v>
+        <v>372</v>
       </c>
       <c r="H57" t="s">
-        <v>178</v>
+        <v>240</v>
       </c>
       <c r="I57" t="s">
-        <v>179</v>
+        <v>241</v>
       </c>
       <c r="J57" t="s">
-        <v>117</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2833,7 +3586,7 @@
         <v>7</v>
       </c>
       <c r="B58" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C58">
         <v>3</v>
@@ -2845,19 +3598,19 @@
         <v>10</v>
       </c>
       <c r="F58" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="G58" t="s">
-        <v>177</v>
+        <v>373</v>
       </c>
       <c r="H58" t="s">
-        <v>178</v>
+        <v>242</v>
       </c>
       <c r="I58" t="s">
-        <v>179</v>
+        <v>243</v>
       </c>
       <c r="J58" t="s">
-        <v>119</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -2865,7 +3618,7 @@
         <v>7</v>
       </c>
       <c r="B59" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C59">
         <v>4</v>
@@ -2877,19 +3630,19 @@
         <v>10</v>
       </c>
       <c r="F59" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="G59" t="s">
-        <v>177</v>
+        <v>374</v>
       </c>
       <c r="H59" t="s">
-        <v>178</v>
+        <v>244</v>
       </c>
       <c r="I59" t="s">
-        <v>179</v>
+        <v>245</v>
       </c>
       <c r="J59" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -2897,7 +3650,7 @@
         <v>7</v>
       </c>
       <c r="B60" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C60">
         <v>5</v>
@@ -2909,19 +3662,19 @@
         <v>10</v>
       </c>
       <c r="F60" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="G60" t="s">
-        <v>177</v>
+        <v>375</v>
       </c>
       <c r="H60" t="s">
-        <v>178</v>
+        <v>376</v>
       </c>
       <c r="I60" t="s">
-        <v>179</v>
+        <v>377</v>
       </c>
       <c r="J60" t="s">
-        <v>123</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -2929,7 +3682,7 @@
         <v>7</v>
       </c>
       <c r="B61" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C61">
         <v>6</v>
@@ -2941,19 +3694,19 @@
         <v>10</v>
       </c>
       <c r="F61" t="s">
-        <v>124</v>
+        <v>165</v>
       </c>
       <c r="G61" t="s">
-        <v>177</v>
+        <v>378</v>
       </c>
       <c r="H61" t="s">
-        <v>178</v>
+        <v>246</v>
       </c>
       <c r="I61" t="s">
-        <v>179</v>
+        <v>379</v>
       </c>
       <c r="J61" t="s">
-        <v>125</v>
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2961,31 +3714,31 @@
         <v>7</v>
       </c>
       <c r="B62" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C62">
         <v>7</v>
       </c>
       <c r="D62" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E62" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F62" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="G62" t="s">
-        <v>177</v>
+        <v>380</v>
       </c>
       <c r="H62" t="s">
-        <v>178</v>
+        <v>381</v>
       </c>
       <c r="I62" t="s">
-        <v>179</v>
+        <v>382</v>
       </c>
       <c r="J62" t="s">
-        <v>127</v>
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2993,31 +3746,31 @@
         <v>7</v>
       </c>
       <c r="B63" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C63">
         <v>8</v>
       </c>
       <c r="D63" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E63" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F63" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="G63" t="s">
-        <v>177</v>
+        <v>383</v>
       </c>
       <c r="H63" t="s">
-        <v>178</v>
+        <v>384</v>
       </c>
       <c r="I63" t="s">
-        <v>179</v>
+        <v>385</v>
       </c>
       <c r="J63" t="s">
-        <v>129</v>
+        <v>80</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -3025,31 +3778,31 @@
         <v>7</v>
       </c>
       <c r="B64" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C64">
         <v>9</v>
       </c>
       <c r="D64" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E64" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F64" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="G64" t="s">
-        <v>177</v>
+        <v>386</v>
       </c>
       <c r="H64" t="s">
-        <v>178</v>
+        <v>247</v>
       </c>
       <c r="I64" t="s">
-        <v>179</v>
+        <v>248</v>
       </c>
       <c r="J64" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -3057,31 +3810,31 @@
         <v>7</v>
       </c>
       <c r="B65" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C65">
         <v>10</v>
       </c>
       <c r="D65" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E65" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F65" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="G65" t="s">
-        <v>177</v>
+        <v>387</v>
       </c>
       <c r="H65" t="s">
-        <v>178</v>
+        <v>249</v>
       </c>
       <c r="I65" t="s">
-        <v>179</v>
+        <v>250</v>
       </c>
       <c r="J65" t="s">
-        <v>133</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -3089,31 +3842,31 @@
         <v>7</v>
       </c>
       <c r="B66" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C66">
         <v>11</v>
       </c>
       <c r="D66" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E66" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F66" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="G66" t="s">
-        <v>177</v>
+        <v>388</v>
       </c>
       <c r="H66" t="s">
-        <v>178</v>
+        <v>389</v>
       </c>
       <c r="I66" t="s">
-        <v>179</v>
+        <v>390</v>
       </c>
       <c r="J66" t="s">
-        <v>135</v>
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -3121,31 +3874,31 @@
         <v>7</v>
       </c>
       <c r="B67" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C67">
         <v>12</v>
       </c>
       <c r="D67" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E67" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F67" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="G67" t="s">
-        <v>177</v>
+        <v>391</v>
       </c>
       <c r="H67" t="s">
-        <v>178</v>
+        <v>392</v>
       </c>
       <c r="I67" t="s">
-        <v>179</v>
+        <v>393</v>
       </c>
       <c r="J67" t="s">
-        <v>137</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -3153,31 +3906,31 @@
         <v>7</v>
       </c>
       <c r="B68" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C68">
         <v>13</v>
       </c>
       <c r="D68" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E68" t="s">
         <v>10</v>
       </c>
       <c r="F68" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="G68" t="s">
-        <v>177</v>
+        <v>394</v>
       </c>
       <c r="H68" t="s">
-        <v>178</v>
+        <v>395</v>
       </c>
       <c r="I68" t="s">
-        <v>179</v>
+        <v>396</v>
       </c>
       <c r="J68" t="s">
-        <v>139</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -3185,31 +3938,31 @@
         <v>7</v>
       </c>
       <c r="B69" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C69">
         <v>14</v>
       </c>
       <c r="D69" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E69" t="s">
         <v>10</v>
       </c>
       <c r="F69" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="G69" t="s">
-        <v>177</v>
+        <v>397</v>
       </c>
       <c r="H69" t="s">
-        <v>178</v>
+        <v>398</v>
       </c>
       <c r="I69" t="s">
-        <v>179</v>
+        <v>399</v>
       </c>
       <c r="J69" t="s">
-        <v>141</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -3217,31 +3970,31 @@
         <v>7</v>
       </c>
       <c r="B70" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C70">
         <v>15</v>
       </c>
       <c r="D70" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E70" t="s">
         <v>10</v>
       </c>
       <c r="F70" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="G70" t="s">
-        <v>177</v>
+        <v>400</v>
       </c>
       <c r="H70" t="s">
-        <v>178</v>
+        <v>251</v>
       </c>
       <c r="I70" t="s">
-        <v>179</v>
+        <v>252</v>
       </c>
       <c r="J70" t="s">
-        <v>143</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -3249,31 +4002,31 @@
         <v>7</v>
       </c>
       <c r="B71" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C71">
         <v>16</v>
       </c>
       <c r="D71" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E71" t="s">
         <v>10</v>
       </c>
       <c r="F71" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="G71" t="s">
-        <v>177</v>
+        <v>401</v>
       </c>
       <c r="H71" t="s">
-        <v>178</v>
+        <v>402</v>
       </c>
       <c r="I71" t="s">
-        <v>179</v>
+        <v>403</v>
       </c>
       <c r="J71" t="s">
-        <v>145</v>
+        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -3281,31 +4034,31 @@
         <v>7</v>
       </c>
       <c r="B72" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C72">
         <v>17</v>
       </c>
       <c r="D72" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E72" t="s">
         <v>10</v>
       </c>
       <c r="F72" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="G72" t="s">
-        <v>177</v>
+        <v>404</v>
       </c>
       <c r="H72" t="s">
-        <v>178</v>
+        <v>253</v>
       </c>
       <c r="I72" t="s">
-        <v>179</v>
+        <v>254</v>
       </c>
       <c r="J72" t="s">
-        <v>147</v>
+        <v>89</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -3313,36 +4066,36 @@
         <v>7</v>
       </c>
       <c r="B73" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C73">
         <v>18</v>
       </c>
       <c r="D73" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E73" t="s">
         <v>10</v>
       </c>
       <c r="F73" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="G73" t="s">
-        <v>177</v>
+        <v>405</v>
       </c>
       <c r="H73" t="s">
-        <v>178</v>
+        <v>255</v>
       </c>
       <c r="I73" t="s">
-        <v>179</v>
+        <v>256</v>
       </c>
       <c r="J73" t="s">
-        <v>149</v>
+        <v>90</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B74" t="s">
         <v>8</v>
@@ -3357,24 +4110,24 @@
         <v>10</v>
       </c>
       <c r="F74" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="G74" t="s">
-        <v>177</v>
+        <v>257</v>
       </c>
       <c r="H74" t="s">
-        <v>178</v>
+        <v>406</v>
       </c>
       <c r="I74" t="s">
-        <v>179</v>
+        <v>258</v>
       </c>
       <c r="J74" t="s">
-        <v>151</v>
+        <v>91</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B75" t="s">
         <v>8</v>
@@ -3383,33 +4136,33 @@
         <v>2</v>
       </c>
       <c r="D75" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E75" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F75" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="G75" t="s">
-        <v>177</v>
+        <v>407</v>
       </c>
       <c r="H75" t="s">
-        <v>178</v>
+        <v>408</v>
       </c>
       <c r="I75" t="s">
-        <v>179</v>
+        <v>409</v>
       </c>
       <c r="J75" t="s">
-        <v>153</v>
+        <v>92</v>
       </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B76" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -3421,59 +4174,59 @@
         <v>10</v>
       </c>
       <c r="F76" t="s">
-        <v>154</v>
+        <v>93</v>
       </c>
       <c r="G76" t="s">
-        <v>177</v>
+        <v>259</v>
       </c>
       <c r="H76" t="s">
-        <v>178</v>
+        <v>260</v>
       </c>
       <c r="I76" t="s">
-        <v>179</v>
+        <v>261</v>
       </c>
       <c r="J76" t="s">
-        <v>155</v>
+        <v>94</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B77" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C77">
         <v>2</v>
       </c>
       <c r="D77" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E77" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F77" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G77" t="s">
-        <v>177</v>
+        <v>262</v>
       </c>
       <c r="H77" t="s">
-        <v>178</v>
+        <v>410</v>
       </c>
       <c r="I77" t="s">
-        <v>179</v>
+        <v>263</v>
       </c>
       <c r="J77" t="s">
-        <v>157</v>
+        <v>95</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B78" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -3485,91 +4238,91 @@
         <v>10</v>
       </c>
       <c r="F78" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G78" t="s">
-        <v>177</v>
+        <v>411</v>
       </c>
       <c r="H78" t="s">
-        <v>178</v>
+        <v>412</v>
       </c>
       <c r="I78" t="s">
-        <v>179</v>
+        <v>413</v>
       </c>
       <c r="J78" t="s">
-        <v>159</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B79" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C79">
         <v>2</v>
       </c>
       <c r="D79" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E79" t="s">
         <v>10</v>
       </c>
       <c r="F79" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G79" t="s">
-        <v>177</v>
+        <v>414</v>
       </c>
       <c r="H79" t="s">
-        <v>178</v>
+        <v>264</v>
       </c>
       <c r="I79" t="s">
-        <v>179</v>
+        <v>265</v>
       </c>
       <c r="J79" t="s">
-        <v>161</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B80" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E80" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F80" t="s">
         <v>162</v>
       </c>
       <c r="G80" t="s">
-        <v>177</v>
+        <v>415</v>
       </c>
       <c r="H80" t="s">
-        <v>178</v>
+        <v>416</v>
       </c>
       <c r="I80" t="s">
-        <v>179</v>
+        <v>417</v>
       </c>
       <c r="J80" t="s">
-        <v>163</v>
+        <v>98</v>
       </c>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B81" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C81">
         <v>2</v>
@@ -3581,24 +4334,23 @@
         <v>10</v>
       </c>
       <c r="F81" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G81" t="s">
-        <v>177</v>
+        <v>418</v>
       </c>
       <c r="H81" t="s">
-        <v>178</v>
+        <v>266</v>
       </c>
       <c r="I81" t="s">
-        <v>179</v>
+        <v>267</v>
       </c>
       <c r="J81" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>